<commit_message>
added some docs and outputs
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\zaloha\Google Drive\Documents\_škola\bakalarka\_vyvoj\sekvencer\HW\sekvencer_v0.01 HW\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D9092C-21DD-44AB-8006-FED3CAE98E76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1461B2A-E53A-47CB-A4AB-54248D160444}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21468" windowHeight="9084" xr2:uid="{C3DC6A11-751E-43E4-9C23-7B39ED2EC226}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7644" xr2:uid="{C3DC6A11-751E-43E4-9C23-7B39ED2EC226}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -3141,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN754"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H67" workbookViewId="0">
-      <selection activeCell="Q75" sqref="Q75"/>
+    <sheetView tabSelected="1" topLeftCell="C85" workbookViewId="0">
+      <selection activeCell="P96" sqref="P96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8880,7 +8880,7 @@
         <v>746</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="P100" s="1" t="s">
         <v>189</v>
@@ -8889,7 +8889,7 @@
         <v>253</v>
       </c>
       <c r="R100" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="S100" s="1" t="s">
         <v>295</v>
@@ -8904,7 +8904,7 @@
         <v>44</v>
       </c>
       <c r="W100" s="1" t="s">
-        <v>332</v>
+        <v>373</v>
       </c>
       <c r="X100" s="1"/>
       <c r="Y100" s="1"/>
@@ -8939,7 +8939,7 @@
         <v>746</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="P101" s="1" t="s">
         <v>189</v>
@@ -8963,7 +8963,7 @@
         <v>44</v>
       </c>
       <c r="W101" s="1" t="s">
-        <v>381</v>
+        <v>332</v>
       </c>
       <c r="X101" s="1"/>
       <c r="Y101" s="1"/>
@@ -8998,7 +8998,7 @@
         <v>746</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="P102" s="1" t="s">
         <v>189</v>
@@ -9007,7 +9007,7 @@
         <v>253</v>
       </c>
       <c r="R102" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="S102" s="1" t="s">
         <v>295</v>
@@ -9022,7 +9022,7 @@
         <v>44</v>
       </c>
       <c r="W102" s="1" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="X102" s="1"/>
       <c r="Y102" s="1"/>
@@ -41843,14 +41843,14 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R89" r:id="rId1" xr:uid="{CA12F73E-44C5-4324-8FC8-A9B57D38C99D}"/>
-    <hyperlink ref="R100" r:id="rId2" xr:uid="{64A4FD5B-77EE-402D-AEB8-EEC7B4AEAB4F}"/>
+    <hyperlink ref="R101" r:id="rId2" xr:uid="{64A4FD5B-77EE-402D-AEB8-EEC7B4AEAB4F}"/>
     <hyperlink ref="R109" r:id="rId3" xr:uid="{84C9D1D1-AF8D-44A2-87A7-FE6F12DA721B}"/>
     <hyperlink ref="R5" r:id="rId4" xr:uid="{46A6E6CC-E647-41F3-846A-81F4C486B9B3}"/>
     <hyperlink ref="R4" r:id="rId5" xr:uid="{4A39D377-F087-4412-83E0-01FC2E519A54}"/>
     <hyperlink ref="R91" r:id="rId6" xr:uid="{588F2E4E-BC27-404B-8D06-425E4747C284}"/>
-    <hyperlink ref="R102" r:id="rId7" xr:uid="{863DB97C-F3B9-4B13-B8E4-7B51C771260B}"/>
+    <hyperlink ref="R100" r:id="rId7" xr:uid="{863DB97C-F3B9-4B13-B8E4-7B51C771260B}"/>
     <hyperlink ref="R123" r:id="rId8" xr:uid="{41391F62-86A8-46B8-AB2C-501227609038}"/>
-    <hyperlink ref="R101" r:id="rId9" xr:uid="{C7BEB470-DAC2-4922-B0A9-CB1F42E9AA52}"/>
+    <hyperlink ref="R102" r:id="rId9" xr:uid="{C7BEB470-DAC2-4922-B0A9-CB1F42E9AA52}"/>
     <hyperlink ref="R125" r:id="rId10" xr:uid="{1B59E611-2748-4EC3-9027-9086673242B8}"/>
     <hyperlink ref="R126" r:id="rId11" xr:uid="{55478C83-46B6-4A1C-B86C-68228E812252}"/>
     <hyperlink ref="R120" r:id="rId12" xr:uid="{32BF538D-1B41-4612-AD47-4D673119D3C1}"/>

</xml_diff>